<commit_message>
Learning Moves by Gaining Xp from battle. Forgetting Move and Learning new Move System and Move Selection UI Implement
</commit_message>
<xml_diff>
--- a/Assets/Proje.xlsx
+++ b/Assets/Proje.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28922"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/A622EF9FF3752AA9/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Game_Projects\PokemonProject\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8E43331-4521-4449-A966-5F423F8C4F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936DF4A8-42A1-4797-93C5-D2DA4E167165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E67DA6A6-E460-427A-A371-FC47EFBADD69}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="81">
   <si>
     <t>Yapılması Planlananlar</t>
   </si>
@@ -264,13 +262,28 @@
   </si>
   <si>
     <t>Biraz daha aktif NPCler ve kullanılabilir dünya</t>
+  </si>
+  <si>
+    <t>Pokemon Sistemi DataBase'e entegre edilecek</t>
+  </si>
+  <si>
+    <t>Pokemon oluşturmak ScriptibleObject yerine JSON temelli olacak</t>
+  </si>
+  <si>
+    <t>Shiny Pokemon</t>
+  </si>
+  <si>
+    <t>Shiny sistemi eklenecek</t>
+  </si>
+  <si>
+    <t>Pokemon sistemi oturduktan sonra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,7 +361,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -644,21 +657,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134A7531-8AAC-4727-89CB-316374D3B977}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="50.28515625" customWidth="1"/>
+    <col min="1" max="1" width="37.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="53.109375" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -686,7 +699,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -700,7 +713,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -714,7 +727,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -728,7 +741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -742,7 +755,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -756,7 +769,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -770,7 +783,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -784,7 +797,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -798,7 +811,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -812,7 +825,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -826,7 +839,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -840,7 +853,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -854,7 +867,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -868,7 +881,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -882,7 +895,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -896,7 +909,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -910,7 +923,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -924,7 +937,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -938,7 +951,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -952,7 +965,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -966,7 +979,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>60</v>
       </c>
@@ -980,7 +993,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>62</v>
       </c>
@@ -994,7 +1007,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -1008,7 +1021,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>67</v>
       </c>
@@ -1022,7 +1035,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>69</v>
       </c>
@@ -1036,7 +1049,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -1050,7 +1063,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>73</v>
       </c>
@@ -1062,6 +1075,34 @@
       </c>
       <c r="D29" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Implement quest system with quest management and item database
- Added Quest and QuestBase classes to manage quests and their states.
- Integrated quest handling in NPCController for starting and completing quests.
- Created ItemDB for managing items and their retrieval.
- Updated PlayerController to handle player interactions with triggerable objects.
- Enhanced inventory system to support saving and restoring state.
- Introduced IPlayerTriggerable interface for consistent triggerable behavior.
- Added LongGrass and StoryItem classes as examples of triggerable objects.
- Updated GameLayers to include triggers layer for better collision management.
- Implemented ItemGiver and PickUp classes for item distribution and collection.
- Added meta files for new scripts and assets.
</commit_message>
<xml_diff>
--- a/Assets/Proje.xlsx
+++ b/Assets/Proje.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Game_Projects\PokemonProject\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936DF4A8-42A1-4797-93C5-D2DA4E167165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7BACF9-F1D6-45AE-8526-B1DEE6B239AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E67DA6A6-E460-427A-A371-FC47EFBADD69}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="92">
   <si>
     <t>Yapılması Planlananlar</t>
   </si>
@@ -277,6 +277,39 @@
   </si>
   <si>
     <t>Pokemon sistemi oturduktan sonra</t>
+  </si>
+  <si>
+    <t>Pidgey Delivery</t>
+  </si>
+  <si>
+    <t>Mağaza</t>
+  </si>
+  <si>
+    <t>Biraz daha fazla fiyata istediğin yere sipariş getiren bir kurye firması</t>
+  </si>
+  <si>
+    <t>Shop UI düzenlemesi</t>
+  </si>
+  <si>
+    <t>Daha gerçekçi bir alışveriş matığı, reondan sepete ekleyip kasada ödeme.()</t>
+  </si>
+  <si>
+    <t>Quest UI</t>
+  </si>
+  <si>
+    <t>Görevler</t>
+  </si>
+  <si>
+    <t>Oyuncunun görevlerini takip edebilmesi için</t>
+  </si>
+  <si>
+    <t>Character DialogBox</t>
+  </si>
+  <si>
+    <t>Diaog</t>
+  </si>
+  <si>
+    <t>Her karakterin üzerinde kendi konuşmalarına özel dialogboxlar olur karakterler onların üzerinden konuşur.</t>
   </si>
 </sst>
 </file>
@@ -337,12 +370,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -657,457 +701,513 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134A7531-8AAC-4727-89CB-316374D3B977}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.77734375" customWidth="1"/>
     <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="3" max="3" width="53.109375" customWidth="1"/>
+    <col min="3" max="3" width="88.21875" customWidth="1"/>
     <col min="4" max="4" width="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="D12" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="D13" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="D14" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="D15" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="D16" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="D17" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="D18" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="D19" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="D20" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="D21" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D21" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="D22" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D22" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="D23" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="D24" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="D25" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D25" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="D26" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="D27" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D27" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="D28" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="D29" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D29" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="D30" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" t="s">
-        <v>79</v>
-      </c>
-      <c r="D31" t="s">
-        <v>80</v>
+      <c r="D31" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D29">
-    <sortCondition descending="1" ref="D2:D29"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D35">
+    <sortCondition descending="1" ref="D7:D35"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>